<commit_message>
changes in .xlsx files
</commit_message>
<xml_diff>
--- a/task_2/test_case_document.xlsx
+++ b/task_2/test_case_document.xlsx
@@ -611,10 +611,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="A8" sqref="A8"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>